<commit_message>
edited some of the excel sheets
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/Frames/Train/total frames.xlsx
+++ b/Dataset Excel Sheets/Frames/Train/total frames.xlsx
@@ -10,26 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.0" hidden="1">Sheet1!$A$1:$A$3811</definedName>
-    <definedName name="_xlchart.1" hidden="1">Sheet1!$B$1:$B$3811</definedName>
-    <definedName name="_xlchart.10" hidden="1">Sheet1!$C$1:$C$3811</definedName>
-    <definedName name="_xlchart.11" hidden="1">Sheet1!$D$1:$D$3811</definedName>
-    <definedName name="_xlchart.12" hidden="1">Sheet1!$A$1:$A$3811</definedName>
-    <definedName name="_xlchart.13" hidden="1">Sheet1!$B$1:$B$3811</definedName>
-    <definedName name="_xlchart.14" hidden="1">Sheet1!$C$1:$C$3811</definedName>
-    <definedName name="_xlchart.15" hidden="1">Sheet1!$D$1:$D$3811</definedName>
-    <definedName name="_xlchart.16" hidden="1">Sheet1!$A$1:$A$3811</definedName>
-    <definedName name="_xlchart.17" hidden="1">Sheet1!$B$1:$B$3811</definedName>
-    <definedName name="_xlchart.18" hidden="1">Sheet1!$C$1:$C$3811</definedName>
-    <definedName name="_xlchart.19" hidden="1">Sheet1!$D$1:$D$3811</definedName>
-    <definedName name="_xlchart.2" hidden="1">Sheet1!$C$1:$C$3811</definedName>
-    <definedName name="_xlchart.3" hidden="1">Sheet1!$D$1:$D$3811</definedName>
+    <definedName name="_xlchart.0" hidden="1">Sheet1!$A$2:$A$3811</definedName>
+    <definedName name="_xlchart.1" hidden="1">Sheet1!$B$2:$B$3811</definedName>
+    <definedName name="_xlchart.2" hidden="1">Sheet1!$C$2:$C$3811</definedName>
+    <definedName name="_xlchart.3" hidden="1">Sheet1!$D$2:$D$3811</definedName>
     <definedName name="_xlchart.4" hidden="1">Sheet1!$A$2:$A$3811</definedName>
     <definedName name="_xlchart.5" hidden="1">Sheet1!$B$2:$B$3811</definedName>
     <definedName name="_xlchart.6" hidden="1">Sheet1!$C$2:$C$3811</definedName>
     <definedName name="_xlchart.7" hidden="1">Sheet1!$D$2:$D$3811</definedName>
-    <definedName name="_xlchart.8" hidden="1">Sheet1!$A$1:$A$3811</definedName>
-    <definedName name="_xlchart.9" hidden="1">Sheet1!$B$1:$B$3811</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -388,7 +376,7 @@
         </cx:series>
       </cx:plotAreaRegion>
       <cx:axis id="0">
-        <cx:catScaling gapWidth="1"/>
+        <cx:catScaling gapWidth="1.5"/>
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
@@ -397,7 +385,9 @@
         <cx:tickLabels/>
       </cx:axis>
     </cx:plotArea>
+    <cx:legend pos="b" align="ctr" overlay="0"/>
   </cx:chart>
+  <cx:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
 </cx:chartSpace>
 </file>
 
@@ -442,15 +432,15 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="408">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900"/>
@@ -460,56 +450,72 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="-60000000" vert="horz"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900"/>
@@ -519,23 +525,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -571,12 +573,20 @@
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -604,20 +614,18 @@
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr"/>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:alpha val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -625,7 +633,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="28575" cap="rnd">
@@ -641,17 +649,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -663,18 +671,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -688,7 +696,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:dropLine>
   <cs:errorBar>
@@ -696,7 +704,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:errorBar>
   <cs:floor>
@@ -704,7 +712,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -712,16 +720,28 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -731,17 +751,30 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-            <a:lumOff val="10000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+                <a:lumOff val="10000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+                <a:lumOff val="10000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -750,14 +783,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -769,7 +802,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:leaderLine>
   <cs:legend>
@@ -777,27 +810,35 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
     <cs:defRPr sz="900"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -805,17 +846,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -829,7 +870,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat">
@@ -845,12 +886,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
     <cs:bodyPr rot="0" vert="horz"/>
   </cs:title>
   <cs:trendline>
@@ -858,7 +899,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
@@ -874,9 +915,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900"/>
@@ -886,7 +927,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -894,9 +935,8 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -908,9 +948,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -921,7 +961,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -1265,8 +1305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3811"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="77" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added the ranges of predicting frames
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/Frames/Train/total frames.xlsx
+++ b/Dataset Excel Sheets/Frames/Train/total frames.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>2 words</t>
   </si>
@@ -98,6 +98,27 @@
   </si>
   <si>
     <t>[94-311]</t>
+  </si>
+  <si>
+    <t>&gt;=148</t>
+  </si>
+  <si>
+    <t>&lt;=98</t>
+  </si>
+  <si>
+    <t>(98,132]</t>
+  </si>
+  <si>
+    <t>[133, 147]</t>
+  </si>
+  <si>
+    <t>&gt;=133 [133, 239]</t>
+  </si>
+  <si>
+    <t>ranges with 5</t>
+  </si>
+  <si>
+    <t>ranges without 5</t>
   </si>
 </sst>
 </file>
@@ -266,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -301,6 +322,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -323,30 +345,51 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.4</cx:f>
+        <cx:f>_xlchart.0</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.5</cx:f>
+        <cx:f>_xlchart.1</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.6</cx:f>
+        <cx:f>_xlchart.2</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.7</cx:f>
+        <cx:f>_xlchart.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>No. Frames Per No. Words</a:t>
+            </a:r>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:series layoutId="boxWhisker" uniqueId="{7E947D06-DB6F-47D0-B9AD-75FB4E8269BC}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>2 words</cx:v>
+            </cx:txData>
+          </cx:tx>
           <cx:dataId val="0"/>
           <cx:layoutPr>
             <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
@@ -354,6 +397,11 @@
           </cx:layoutPr>
         </cx:series>
         <cx:series layoutId="boxWhisker" uniqueId="{9DA63BCD-CB51-4591-BC4D-D22414C8D407}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>3 words</cx:v>
+            </cx:txData>
+          </cx:tx>
           <cx:dataId val="1"/>
           <cx:layoutPr>
             <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
@@ -361,6 +409,11 @@
           </cx:layoutPr>
         </cx:series>
         <cx:series layoutId="boxWhisker" uniqueId="{A7F4A66C-5780-4B98-B921-499079A2FEC8}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>4 words</cx:v>
+            </cx:txData>
+          </cx:tx>
           <cx:dataId val="2"/>
           <cx:layoutPr>
             <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
@@ -368,6 +421,11 @@
           </cx:layoutPr>
         </cx:series>
         <cx:series layoutId="boxWhisker" uniqueId="{A56984BA-EEBA-47E1-9F49-E2F4B8632643}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>5 words</cx:v>
+            </cx:txData>
+          </cx:tx>
           <cx:dataId val="3"/>
           <cx:layoutPr>
             <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
@@ -375,7 +433,7 @@
           </cx:layoutPr>
         </cx:series>
       </cx:plotAreaRegion>
-      <cx:axis id="0">
+      <cx:axis id="0" hidden="1">
         <cx:catScaling gapWidth="1.5"/>
         <cx:tickLabels/>
       </cx:axis>
@@ -1305,14 +1363,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3811"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="77" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="7" max="10" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="39.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1595,8 +1654,14 @@
         <f t="shared" si="5"/>
         <v>167</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
@@ -1637,6 +1702,12 @@
       <c r="M9" t="s">
         <v>19</v>
       </c>
+      <c r="N9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10">
@@ -1676,6 +1747,12 @@
       <c r="M10" t="s">
         <v>20</v>
       </c>
+      <c r="N10" t="s">
+        <v>25</v>
+      </c>
+      <c r="O10" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -1696,6 +1773,12 @@
       <c r="M11" t="s">
         <v>21</v>
       </c>
+      <c r="N11" t="s">
+        <v>26</v>
+      </c>
+      <c r="O11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12">
@@ -1716,6 +1799,9 @@
       <c r="M12" t="s">
         <v>22</v>
       </c>
+      <c r="N12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -1744,6 +1830,7 @@
       <c r="D14">
         <v>190</v>
       </c>
+      <c r="L14" s="14"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15">

</xml_diff>